<commit_message>
fix bills,bill in page customer
</commit_message>
<xml_diff>
--- a/public/excels/exports/Re2021-export.xlsx
+++ b/public/excels/exports/Re2021-export.xlsx
@@ -1504,7 +1504,7 @@
       </c>
       <c r="J24" s="26">
         <f>SUM(J26:J27)</f>
-        <v>1.65984</v>
+        <v>0</v>
       </c>
       <c r="K24" s="58" t="s">
         <v>29</v>
@@ -1633,7 +1633,7 @@
         <v>756.0</v>
       </c>
       <c r="J27" s="19">
-        <v>1.65984</v>
+        <v>0</v>
       </c>
       <c r="K27" s="19">
         <v>14</v>
@@ -1720,7 +1720,7 @@
         <v>6420.0</v>
       </c>
       <c r="J29" s="19">
-        <v>13.0572</v>
+        <v>0</v>
       </c>
       <c r="K29" s="19">
         <v>18</v>
@@ -1763,7 +1763,7 @@
         <v>2448.0</v>
       </c>
       <c r="J30" s="19">
-        <v>7.49232</v>
+        <v>0</v>
       </c>
       <c r="K30" s="19">
         <v>11</v>
@@ -1806,7 +1806,7 @@
         <v>2300.0</v>
       </c>
       <c r="J31" s="19">
-        <v>5.265</v>
+        <v>0</v>
       </c>
       <c r="K31" s="19">
         <v>25</v>
@@ -1849,7 +1849,7 @@
         <v>7008.0</v>
       </c>
       <c r="J32" s="19">
-        <v>21.63168</v>
+        <v>0</v>
       </c>
       <c r="K32" s="19">
         <v>21</v>

</xml_diff>